<commit_message>
HW1 Campaign RU Spreadsheet Update
</commit_message>
<xml_diff>
--- a/BalanceInfo/2.3 HW1 Campaign RU.xlsx
+++ b/BalanceInfo/2.3 HW1 Campaign RU.xlsx
@@ -17,18 +17,19 @@
     <sheet name="M2" sheetId="1" r:id="rId3"/>
     <sheet name="M3" sheetId="3" r:id="rId4"/>
     <sheet name="M4" sheetId="6" r:id="rId5"/>
-    <sheet name="M5" sheetId="7" r:id="rId6"/>
-    <sheet name="M6" sheetId="8" r:id="rId7"/>
-    <sheet name="M7" sheetId="10" r:id="rId8"/>
-    <sheet name="M8" sheetId="11" r:id="rId9"/>
-    <sheet name="M9" sheetId="12" r:id="rId10"/>
-    <sheet name="M10" sheetId="13" r:id="rId11"/>
-    <sheet name="M11" sheetId="14" r:id="rId12"/>
-    <sheet name="M12" sheetId="15" r:id="rId13"/>
-    <sheet name="M13" sheetId="16" r:id="rId14"/>
-    <sheet name="M14" sheetId="17" r:id="rId15"/>
-    <sheet name="M15" sheetId="18" r:id="rId16"/>
-    <sheet name="M16" sheetId="19" r:id="rId17"/>
+    <sheet name="M4.5" sheetId="20" r:id="rId6"/>
+    <sheet name="M5" sheetId="7" r:id="rId7"/>
+    <sheet name="M6" sheetId="8" r:id="rId8"/>
+    <sheet name="M7" sheetId="10" r:id="rId9"/>
+    <sheet name="M8" sheetId="11" r:id="rId10"/>
+    <sheet name="M9" sheetId="12" r:id="rId11"/>
+    <sheet name="M10" sheetId="13" r:id="rId12"/>
+    <sheet name="M11" sheetId="14" r:id="rId13"/>
+    <sheet name="M12" sheetId="15" r:id="rId14"/>
+    <sheet name="M13" sheetId="16" r:id="rId15"/>
+    <sheet name="M14" sheetId="17" r:id="rId16"/>
+    <sheet name="M15" sheetId="18" r:id="rId17"/>
+    <sheet name="M16" sheetId="19" r:id="rId18"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="47">
   <si>
     <t>b8</t>
   </si>
@@ -123,12 +124,6 @@
     <t>Total Asteriods</t>
   </si>
   <si>
-    <t>Mission First Available</t>
-  </si>
-  <si>
-    <t>Free in SP</t>
-  </si>
-  <si>
     <t>no changes</t>
   </si>
   <si>
@@ -147,16 +142,46 @@
     <t>b8 Cost</t>
   </si>
   <si>
-    <t>Desired Mission RU Change</t>
-  </si>
-  <si>
     <t>HW1 Campaign Research</t>
   </si>
   <si>
-    <t>Research Cost Change</t>
-  </si>
-  <si>
     <t>1 in hw1c</t>
+  </si>
+  <si>
+    <t>Special Notes</t>
+  </si>
+  <si>
+    <t>4.5 in Raiders Retreat</t>
+  </si>
+  <si>
+    <t>4.5 Raiders Retreat</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Its Free</t>
+  </si>
+  <si>
+    <t>4 from Bentusi for less ru</t>
+  </si>
+  <si>
+    <t>6 from Bentusi for less ru</t>
+  </si>
+  <si>
+    <t>Potentially get in 9 for Free. M12 is full price.</t>
+  </si>
+  <si>
+    <t>Mission Available</t>
+  </si>
+  <si>
+    <t>Cost Change</t>
+  </si>
+  <si>
+    <t>Desired Level RU Change</t>
+  </si>
+  <si>
+    <t>2.205 to WIP Level RU Change</t>
   </si>
 </sst>
 </file>
@@ -180,12 +205,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -200,10 +231,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -484,50 +516,57 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.7109375" customWidth="1"/>
-    <col min="9" max="9" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="12.7109375" customWidth="1"/>
+    <col min="11" max="11" width="23" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="J1" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -537,26 +576,35 @@
       <c r="C2" s="1">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2">
+      <c r="D2" s="1">
         <v>1</v>
       </c>
+      <c r="E2" t="s">
+        <v>39</v>
+      </c>
       <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
         <f>B3</f>
         <v>200</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <f>C3</f>
         <v>800</v>
       </c>
-      <c r="I2">
-        <f>H2-G2</f>
+      <c r="J2">
+        <f>I2-H2</f>
         <v>600</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2">
+        <v>1500</v>
+      </c>
+      <c r="L2" s="3">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -566,14 +614,32 @@
       <c r="C3" s="1">
         <v>800</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>1</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <f>SUM(B7:B9)</f>
+        <v>1200</v>
+      </c>
+      <c r="I3">
+        <f>SUM(C7:C9)</f>
+        <v>3300</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J18" si="0">I3-H3</f>
+        <v>2100</v>
+      </c>
+      <c r="K3">
+        <v>2247</v>
+      </c>
+      <c r="L3" s="3">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -583,14 +649,32 @@
       <c r="C4" s="1">
         <v>1000</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>5</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <f>SUM(B12:B13)</f>
+        <v>900</v>
+      </c>
+      <c r="I4">
+        <f>SUM(C12:C13)</f>
+        <v>1500</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>600</v>
+      </c>
+      <c r="K4">
+        <v>100</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -600,14 +684,35 @@
       <c r="C5" s="1">
         <v>1000</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>5</v>
       </c>
-      <c r="F5">
+      <c r="E5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <f>B14/2</f>
+        <v>500</v>
+      </c>
+      <c r="I5">
+        <f>C14/2</f>
+        <v>1000</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -617,11 +722,32 @@
       <c r="C6" s="1">
         <v>1100</v>
       </c>
-      <c r="F6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D6" s="1">
+        <v>12</v>
+      </c>
+      <c r="G6" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6">
+        <f>SUM(B5)</f>
+        <v>400</v>
+      </c>
+      <c r="I6">
+        <f>SUM(C5)</f>
+        <v>1000</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>600</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -631,14 +757,32 @@
       <c r="C7" s="1">
         <v>1500</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>2</v>
       </c>
-      <c r="F7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="H7">
+        <f>SUM(B4:B5)</f>
+        <v>700</v>
+      </c>
+      <c r="I7">
+        <f>SUM(C4:C5)</f>
+        <v>2000</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>1300</v>
+      </c>
+      <c r="K7">
+        <v>595</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -648,14 +792,35 @@
       <c r="C8" s="1">
         <v>1200</v>
       </c>
+      <c r="D8" s="1">
+        <v>2</v>
+      </c>
       <c r="E8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8">
+        <v>6</v>
+      </c>
+      <c r="H8">
+        <f>SUM(B14/2,B15/2,B16)</f>
+        <v>2350</v>
+      </c>
+      <c r="I8">
+        <f>SUM(C14/2,C15/2,C16)</f>
+        <v>3350</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="K8">
+        <v>1582</v>
+      </c>
+      <c r="L8" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -665,11 +830,32 @@
       <c r="C9" s="1">
         <v>600</v>
       </c>
-      <c r="F9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D9" s="1">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>7</v>
+      </c>
+      <c r="H9">
+        <f>SUM(B10)</f>
+        <v>600</v>
+      </c>
+      <c r="I9">
+        <f>SUM(C10)</f>
+        <v>800</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -679,11 +865,32 @@
       <c r="C10" s="1">
         <v>800</v>
       </c>
-      <c r="F10">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D10" s="1">
+        <v>7</v>
+      </c>
+      <c r="G10">
+        <v>8</v>
+      </c>
+      <c r="H10">
+        <f>B15/2</f>
+        <v>550</v>
+      </c>
+      <c r="I10">
+        <f>C15/2</f>
+        <v>650</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
@@ -693,25 +900,70 @@
       <c r="C11" s="1">
         <v>1200</v>
       </c>
-      <c r="F11">
+      <c r="D11" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <v>9</v>
+      </c>
+      <c r="H11">
+        <f>SUM(B17,B22)</f>
+        <v>700</v>
+      </c>
+      <c r="I11">
+        <f>SUM(C17,C22)</f>
+        <v>500</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>-200</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B12" s="1">
-        <v>800</v>
+        <v>0</v>
       </c>
       <c r="C12" s="1">
-        <v>1300</v>
-      </c>
-      <c r="F12">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1">
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12">
+        <v>10</v>
+      </c>
+      <c r="H12">
+        <f>SUM(B11,B20)</f>
+        <v>1000</v>
+      </c>
+      <c r="I12">
+        <f>SUM(C11,C20)</f>
+        <v>1700</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>700</v>
+      </c>
+      <c r="K12">
+        <v>867</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -721,11 +973,30 @@
       <c r="C13" s="1">
         <v>1500</v>
       </c>
-      <c r="F13">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D13" s="1">
+        <v>3</v>
+      </c>
+      <c r="G13">
+        <v>11</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
@@ -735,11 +1006,35 @@
       <c r="C14" s="1">
         <v>2000</v>
       </c>
-      <c r="F14">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D14" s="1">
+        <v>6</v>
+      </c>
+      <c r="E14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14">
+        <v>12</v>
+      </c>
+      <c r="H14">
+        <f>SUM(B6,B18/2)</f>
+        <v>1450</v>
+      </c>
+      <c r="I14">
+        <f>SUM(C6,C18/2)</f>
+        <v>2850</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>1400</v>
+      </c>
+      <c r="K14">
+        <v>600</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
@@ -749,11 +1044,35 @@
       <c r="C15" s="1">
         <v>1300</v>
       </c>
-      <c r="F15">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D15" s="1">
+        <v>8</v>
+      </c>
+      <c r="E15" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15">
+        <v>13</v>
+      </c>
+      <c r="H15">
+        <f>SUM(B19,B23)</f>
+        <v>3700</v>
+      </c>
+      <c r="I15">
+        <f>SUM(C19,C23)</f>
+        <v>9800</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>6100</v>
+      </c>
+      <c r="K15">
+        <v>6008</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
@@ -763,25 +1082,68 @@
       <c r="C16" s="1">
         <v>1700</v>
       </c>
-      <c r="F16">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D16" s="1">
+        <v>6</v>
+      </c>
+      <c r="G16">
+        <v>14</v>
+      </c>
+      <c r="H16">
+        <f>B21</f>
+        <v>150</v>
+      </c>
+      <c r="I16">
+        <f>C21</f>
+        <v>1000</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>850</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B17" s="1">
-        <v>1400</v>
+        <v>0</v>
       </c>
       <c r="C17" s="1">
-        <v>5000</v>
-      </c>
-      <c r="F17">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1">
+        <v>9</v>
+      </c>
+      <c r="E17" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17">
+        <v>15</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
@@ -791,8 +1153,33 @@
       <c r="C18" s="1">
         <v>3500</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D18" s="1">
+        <v>12</v>
+      </c>
+      <c r="E18" t="s">
+        <v>42</v>
+      </c>
+      <c r="G18">
+        <v>16</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
@@ -802,30 +1189,39 @@
       <c r="C19" s="1">
         <v>9000</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D19" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1">
+        <v>300</v>
+      </c>
+      <c r="C20" s="1">
+        <v>500</v>
+      </c>
+      <c r="D20" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B21" s="1">
         <v>150</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C21" s="1">
         <v>1000</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="1">
-        <v>300</v>
-      </c>
-      <c r="C21" s="1">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D21" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>13</v>
       </c>
@@ -835,8 +1231,11 @@
       <c r="C22" s="1">
         <v>500</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D22" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>5</v>
       </c>
@@ -846,18 +1245,21 @@
       <c r="C23" s="1">
         <v>800</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D23" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B24">
         <f>SUM(B2:B23)</f>
-        <v>17150</v>
+        <v>14950</v>
       </c>
       <c r="C24">
         <f>SUM(C2:C23)</f>
-        <v>37300</v>
+        <v>31000</v>
       </c>
     </row>
   </sheetData>
@@ -893,7 +1295,7 @@
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -921,76 +1323,6 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E32"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B1" s="2">
-        <v>2.2050000000000001</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2">
-        <v>70</v>
-      </c>
-      <c r="C2">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3">
-        <v>43</v>
-      </c>
-      <c r="C3">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4">
-        <v>70</v>
-      </c>
-      <c r="C4">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B32" s="2">
-        <f>SUM(B2:B31)</f>
-        <v>183</v>
-      </c>
-      <c r="C32" s="2">
-        <f>SUM(C2:C31)</f>
-        <v>1050</v>
-      </c>
-      <c r="D32" s="2">
-        <f t="shared" ref="D32" si="0">SUM(D2:D31)</f>
-        <v>0</v>
-      </c>
-      <c r="E32" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="0" tint="-0.34998626667073579"/>
@@ -1017,7 +1349,7 @@
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1044,11 +1376,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1068,122 +1402,26 @@
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2">
-        <v>375</v>
+        <v>70</v>
       </c>
       <c r="C2">
-        <v>415</v>
+        <v>700</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3">
-        <v>375</v>
+        <v>43</v>
       </c>
       <c r="C3">
-        <v>415</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4">
-        <v>375</v>
+        <v>70</v>
       </c>
       <c r="C4">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5">
-        <v>375</v>
-      </c>
-      <c r="C5">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6">
-        <v>375</v>
-      </c>
-      <c r="C6">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7">
-        <v>375</v>
-      </c>
-      <c r="C7">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8">
-        <v>375</v>
-      </c>
-      <c r="C8">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9">
-        <v>375</v>
-      </c>
-      <c r="C9">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10">
-        <v>375</v>
-      </c>
-      <c r="C10">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11">
-        <v>375</v>
-      </c>
-      <c r="C11">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12">
-        <v>375</v>
-      </c>
-      <c r="C12">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13">
-        <v>375</v>
-      </c>
-      <c r="C13">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14">
-        <v>375</v>
-      </c>
-      <c r="C14">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15">
-        <v>375</v>
-      </c>
-      <c r="C15">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16">
-        <v>375</v>
-      </c>
-      <c r="C16">
-        <v>415</v>
+        <v>175</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1192,17 +1430,23 @@
       </c>
       <c r="B32" s="2">
         <f>SUM(B2:B31)</f>
-        <v>5625</v>
+        <v>183</v>
       </c>
       <c r="C32" s="2">
         <f>SUM(C2:C31)</f>
-        <v>6225</v>
+        <v>1050</v>
       </c>
       <c r="D32" s="2">
         <f t="shared" ref="D32" si="0">SUM(D2:D31)</f>
         <v>0</v>
       </c>
       <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <f>C32-B32</f>
+        <v>867</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1210,149 +1454,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E32"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B1" s="2">
-        <v>2.2050000000000001</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2">
-        <v>216</v>
-      </c>
-      <c r="C2">
-        <v>970</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3">
-        <v>500</v>
-      </c>
-      <c r="C3">
-        <v>970</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4">
-        <v>500</v>
-      </c>
-      <c r="C4">
-        <v>970</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5">
-        <v>100</v>
-      </c>
-      <c r="C5">
-        <v>970</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6">
-        <v>100</v>
-      </c>
-      <c r="C6">
-        <v>970</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7">
-        <v>100</v>
-      </c>
-      <c r="C7">
-        <v>970</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8">
-        <v>500</v>
-      </c>
-      <c r="C8">
-        <v>970</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9">
-        <v>216</v>
-      </c>
-      <c r="C9">
-        <v>970</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10">
-        <v>1400</v>
-      </c>
-      <c r="C10">
-        <v>970</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11">
-        <v>1400</v>
-      </c>
-      <c r="C11">
-        <v>970</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12">
-        <v>500</v>
-      </c>
-      <c r="C12">
-        <v>970</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13">
-        <v>100</v>
-      </c>
-      <c r="C13">
-        <v>970</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B32" s="2">
-        <f>SUM(B2:B31)</f>
-        <v>5632</v>
-      </c>
-      <c r="C32" s="2">
-        <f>SUM(C2:C31)</f>
-        <v>11640</v>
-      </c>
-      <c r="D32" s="2">
-        <f t="shared" ref="D32" si="0">SUM(D2:D31)</f>
-        <v>0</v>
-      </c>
-      <c r="E32" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="0" tint="-0.34998626667073579"/>
@@ -1379,7 +1481,7 @@
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1399,6 +1501,330 @@
         <v>0</v>
       </c>
       <c r="E32" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E33"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="2">
+        <v>2.2050000000000001</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>375</v>
+      </c>
+      <c r="C2">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>375</v>
+      </c>
+      <c r="C3">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>375</v>
+      </c>
+      <c r="C4">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>375</v>
+      </c>
+      <c r="C5">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>375</v>
+      </c>
+      <c r="C6">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>375</v>
+      </c>
+      <c r="C7">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>375</v>
+      </c>
+      <c r="C8">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>375</v>
+      </c>
+      <c r="C9">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>375</v>
+      </c>
+      <c r="C10">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>375</v>
+      </c>
+      <c r="C11">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>375</v>
+      </c>
+      <c r="C12">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>375</v>
+      </c>
+      <c r="C13">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>375</v>
+      </c>
+      <c r="C14">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>375</v>
+      </c>
+      <c r="C15">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>375</v>
+      </c>
+      <c r="C16">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" s="2">
+        <f>SUM(B2:B31)</f>
+        <v>5625</v>
+      </c>
+      <c r="C32" s="2">
+        <f>SUM(C2:C31)</f>
+        <v>6225</v>
+      </c>
+      <c r="D32" s="2">
+        <f t="shared" ref="D32" si="0">SUM(D2:D31)</f>
+        <v>0</v>
+      </c>
+      <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <f>C32-B32</f>
+        <v>600</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E33"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="2">
+        <v>2.2050000000000001</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>216</v>
+      </c>
+      <c r="C2">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>500</v>
+      </c>
+      <c r="C3">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>500</v>
+      </c>
+      <c r="C4">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>100</v>
+      </c>
+      <c r="C5">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>100</v>
+      </c>
+      <c r="C6">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>100</v>
+      </c>
+      <c r="C7">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>500</v>
+      </c>
+      <c r="C8">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>216</v>
+      </c>
+      <c r="C9">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>1400</v>
+      </c>
+      <c r="C10">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>1400</v>
+      </c>
+      <c r="C11">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>500</v>
+      </c>
+      <c r="C12">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>100</v>
+      </c>
+      <c r="C13">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" s="2">
+        <f>SUM(B2:B31)</f>
+        <v>5632</v>
+      </c>
+      <c r="C32" s="2">
+        <f>SUM(C2:C31)</f>
+        <v>11640</v>
+      </c>
+      <c r="D32" s="2">
+        <f t="shared" ref="D32" si="0">SUM(D2:D31)</f>
+        <v>0</v>
+      </c>
+      <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <f>C32-B32</f>
+        <v>6008</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1433,7 +1859,7 @@
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1487,7 +1913,61 @@
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>29</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" s="2">
+        <f>SUM(B2:B31)</f>
+        <v>0</v>
+      </c>
+      <c r="C32" s="2">
+        <f>SUM(C2:C31)</f>
+        <v>0</v>
+      </c>
+      <c r="D32" s="2">
+        <f t="shared" ref="D32" si="0">SUM(D2:D31)</f>
+        <v>0</v>
+      </c>
+      <c r="E32" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="0" tint="-0.34998626667073579"/>
+  </sheetPr>
+  <dimension ref="A1:E32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="2">
+        <v>2.2050000000000001</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1518,7 +1998,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A16" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1638,7 +2118,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2100,7 +2582,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2233,7 +2717,7 @@
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -2261,300 +2745,6 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E32"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B1" s="2">
-        <v>2.2050000000000001</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3">
-        <v>216</v>
-      </c>
-      <c r="C3">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4">
-        <f>B3*84</f>
-        <v>18144</v>
-      </c>
-      <c r="C4">
-        <f>C3*84</f>
-        <v>18732</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B32" s="2">
-        <f>SUM(B2:B31)</f>
-        <v>18360</v>
-      </c>
-      <c r="C32" s="2">
-        <f>SUM(C2:C31)</f>
-        <v>18955</v>
-      </c>
-      <c r="D32" s="2">
-        <f t="shared" ref="D32" si="0">SUM(D2:D31)</f>
-        <v>0</v>
-      </c>
-      <c r="E32" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E32"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B1" s="2">
-        <v>2.2050000000000001</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3">
-        <v>20</v>
-      </c>
-      <c r="C3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4">
-        <v>20</v>
-      </c>
-      <c r="C4">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5">
-        <v>12.5</v>
-      </c>
-      <c r="C5">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6">
-        <v>20</v>
-      </c>
-      <c r="C6">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7">
-        <v>20</v>
-      </c>
-      <c r="C7">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8">
-        <v>12.5</v>
-      </c>
-      <c r="C8">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9">
-        <v>20</v>
-      </c>
-      <c r="C9">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10">
-        <v>12.5</v>
-      </c>
-      <c r="C10">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11">
-        <v>20</v>
-      </c>
-      <c r="C11">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12">
-        <v>20</v>
-      </c>
-      <c r="C12">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13">
-        <v>20</v>
-      </c>
-      <c r="C13">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14">
-        <v>20</v>
-      </c>
-      <c r="C14">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15">
-        <v>20</v>
-      </c>
-      <c r="C15">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16">
-        <v>20</v>
-      </c>
-      <c r="C16">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B18">
-        <v>50</v>
-      </c>
-      <c r="C18">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B19">
-        <v>20</v>
-      </c>
-      <c r="C19">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B20">
-        <v>20</v>
-      </c>
-      <c r="C20">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B21">
-        <v>50</v>
-      </c>
-      <c r="C21">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B22">
-        <v>50</v>
-      </c>
-      <c r="C22">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B23">
-        <v>50</v>
-      </c>
-      <c r="C23">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B24">
-        <v>20</v>
-      </c>
-      <c r="C24">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B32" s="2">
-        <f>SUM(B2:B31)</f>
-        <v>517.5</v>
-      </c>
-      <c r="C32" s="2">
-        <f>SUM(C2:C31)</f>
-        <v>2100</v>
-      </c>
-      <c r="D32" s="2">
-        <f t="shared" ref="D32" si="0">SUM(D2:D31)</f>
-        <v>0</v>
-      </c>
-      <c r="E32" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="0" tint="-0.34998626667073579"/>
@@ -2581,7 +2771,7 @@
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -2593,14 +2783,324 @@
         <v>0</v>
       </c>
       <c r="C32" s="2">
+        <f t="shared" ref="C32:D32" si="0">SUM(C2:C31)</f>
+        <v>0</v>
+      </c>
+      <c r="D32" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E32" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E33"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="2">
+        <v>2.2050000000000001</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>216</v>
+      </c>
+      <c r="C3">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <f>B3*84</f>
+        <v>18144</v>
+      </c>
+      <c r="C4">
+        <f>C3*84</f>
+        <v>18732</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" s="2">
+        <f>SUM(B2:B31)</f>
+        <v>18360</v>
+      </c>
+      <c r="C32" s="2">
         <f>SUM(C2:C31)</f>
-        <v>0</v>
+        <v>18955</v>
       </c>
       <c r="D32" s="2">
         <f t="shared" ref="D32" si="0">SUM(D2:D31)</f>
         <v>0</v>
       </c>
       <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <f>C32-B32</f>
+        <v>595</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E33"/>
+  <sheetViews>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="2">
+        <v>2.2050000000000001</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>12.5</v>
+      </c>
+      <c r="C5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>20</v>
+      </c>
+      <c r="C6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>20</v>
+      </c>
+      <c r="C7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>12.5</v>
+      </c>
+      <c r="C8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>20</v>
+      </c>
+      <c r="C9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>12.5</v>
+      </c>
+      <c r="C10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>20</v>
+      </c>
+      <c r="C11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>20</v>
+      </c>
+      <c r="C12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>20</v>
+      </c>
+      <c r="C13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>20</v>
+      </c>
+      <c r="C14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>20</v>
+      </c>
+      <c r="C15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>20</v>
+      </c>
+      <c r="C16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>50</v>
+      </c>
+      <c r="C18">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>20</v>
+      </c>
+      <c r="C19">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>20</v>
+      </c>
+      <c r="C20">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>50</v>
+      </c>
+      <c r="C21">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>50</v>
+      </c>
+      <c r="C22">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>50</v>
+      </c>
+      <c r="C23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>20</v>
+      </c>
+      <c r="C24">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" s="2">
+        <f>SUM(B2:B31)</f>
+        <v>517.5</v>
+      </c>
+      <c r="C32" s="2">
+        <f>SUM(C2:C31)</f>
+        <v>2100</v>
+      </c>
+      <c r="D32" s="2">
+        <f t="shared" ref="D32" si="0">SUM(D2:D31)</f>
+        <v>0</v>
+      </c>
+      <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <f>C32-B32</f>
+        <v>1582.5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2635,7 +3135,7 @@
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Slight Campaign RU Tweaks
M4.5, 5, 6, 8, and 13. Tried to keep a bit more of the original ru proportions on the later missions.
</commit_message>
<xml_diff>
--- a/BalanceInfo/2.3 HW1 Campaign RU.xlsx
+++ b/BalanceInfo/2.3 HW1 Campaign RU.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="45">
   <si>
     <t>b8</t>
   </si>
@@ -115,9 +115,6 @@
     <t>kus_plasmabomblauncher</t>
   </si>
   <si>
-    <t>echo b8 wip</t>
-  </si>
-  <si>
     <t>Total Research Costs</t>
   </si>
   <si>
@@ -169,9 +166,6 @@
     <t>Potentially get in 9 for Free. M12 is full price.</t>
   </si>
   <si>
-    <t>Mission Available</t>
-  </si>
-  <si>
     <t>Research Cost Change</t>
   </si>
   <si>
@@ -179,6 +173,9 @@
   </si>
   <si>
     <t>Desired 2.205 to WIP Level RU Change</t>
+  </si>
+  <si>
+    <t>diff</t>
   </si>
 </sst>
 </file>
@@ -202,18 +199,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -234,12 +225,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -522,54 +518,52 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="10.7109375" customWidth="1"/>
     <col min="5" max="5" width="41.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="12.7109375" customWidth="1"/>
-    <col min="11" max="11" width="23" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" customWidth="1"/>
+    <col min="11" max="12" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="5"/>
+      <c r="G1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -586,7 +580,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -606,7 +600,7 @@
       <c r="K2">
         <v>1500</v>
       </c>
-      <c r="L2" s="4">
+      <c r="L2" s="3">
         <v>750</v>
       </c>
     </row>
@@ -641,8 +635,8 @@
       <c r="K3">
         <v>2247</v>
       </c>
-      <c r="L3" s="4">
-        <v>2112</v>
+      <c r="L3" s="3">
+        <v>2132</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -676,7 +670,7 @@
       <c r="K4">
         <v>100</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4" s="3">
         <v>669</v>
       </c>
     </row>
@@ -694,7 +688,7 @@
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G5">
         <v>4</v>
@@ -732,7 +726,7 @@
         <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H6">
         <f>SUM(B5)</f>
@@ -750,7 +744,7 @@
         <v>0</v>
       </c>
       <c r="L6" s="3">
-        <v>600</v>
+        <v>500</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -785,7 +779,7 @@
         <v>595</v>
       </c>
       <c r="L7" s="3">
-        <v>1300</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -802,7 +796,7 @@
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G8">
         <v>6</v>
@@ -823,7 +817,7 @@
         <v>1582</v>
       </c>
       <c r="L8" s="3">
-        <v>1000</v>
+        <v>997.5</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -858,7 +852,7 @@
         <v>0</v>
       </c>
       <c r="L9" s="3">
-        <v>200</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -928,7 +922,7 @@
         <v>0</v>
       </c>
       <c r="L11" s="3">
-        <v>-200</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -945,7 +939,7 @@
         <v>3</v>
       </c>
       <c r="E12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G12">
         <v>10</v>
@@ -966,7 +960,7 @@
         <v>867</v>
       </c>
       <c r="L12" s="3">
-        <v>700</v>
+        <v>693</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1016,7 +1010,7 @@
         <v>6</v>
       </c>
       <c r="E14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G14">
         <v>12</v>
@@ -1037,7 +1031,7 @@
         <v>600</v>
       </c>
       <c r="L14" s="3">
-        <v>1400</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -1054,7 +1048,7 @@
         <v>8</v>
       </c>
       <c r="E15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G15">
         <v>13</v>
@@ -1075,7 +1069,7 @@
         <v>6008</v>
       </c>
       <c r="L15" s="3">
-        <v>6100</v>
+        <v>5968</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -1110,7 +1104,7 @@
         <v>0</v>
       </c>
       <c r="L16" s="3">
-        <v>850</v>
+        <v>765</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -1127,7 +1121,7 @@
         <v>9</v>
       </c>
       <c r="E17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G17">
         <v>15</v>
@@ -1163,7 +1157,7 @@
         <v>12</v>
       </c>
       <c r="E18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G18">
         <v>16</v>
@@ -1198,6 +1192,14 @@
       <c r="D19" s="1">
         <v>13</v>
       </c>
+      <c r="J19">
+        <f>SUM(J2:J18)</f>
+        <v>15850</v>
+      </c>
+      <c r="L19">
+        <f>SUM(L2:L18)</f>
+        <v>15744.5</v>
+      </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
@@ -1212,6 +1214,10 @@
       <c r="D20" s="1">
         <v>10</v>
       </c>
+      <c r="L20">
+        <f>L19-J19</f>
+        <v>-105.5</v>
+      </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
@@ -1257,7 +1263,7 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24">
         <f>SUM(B2:B23)</f>
@@ -1277,11 +1283,13 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <tabColor theme="0" tint="-0.34998626667073579"/>
+    <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1300,17 +1308,31 @@
       </c>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>75</v>
+      </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="D2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>75</v>
+      </c>
+      <c r="D3">
+        <v>125</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B32" s="2">
         <f>SUM(B2:B31)</f>
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="C32" s="2">
         <f>SUM(C2:C31)</f>
@@ -1318,9 +1340,15 @@
       </c>
       <c r="D32" s="2">
         <f t="shared" ref="D32" si="0">SUM(D2:D31)</f>
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <f>D32-B32</f>
+        <v>100</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1355,12 +1383,12 @@
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B32" s="2">
         <f>SUM(B2:B31)</f>
@@ -1384,10 +1412,13 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1410,48 +1441,67 @@
       <c r="B2">
         <v>70</v>
       </c>
-      <c r="C2">
-        <v>700</v>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2">
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3">
-        <v>43</v>
-      </c>
-      <c r="C3">
-        <v>175</v>
+        <f>B2*20</f>
+        <v>1400</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="C3:D3" si="0">D2*20</f>
+        <v>2000</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4">
-        <v>70</v>
-      </c>
-      <c r="C4">
-        <v>175</v>
+        <v>43</v>
+      </c>
+      <c r="D4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <f>B4*8</f>
+        <v>344</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ref="C5:D5" si="1">D4*8</f>
+        <v>400</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B32" s="2">
         <f>SUM(B2:B31)</f>
-        <v>183</v>
+        <v>1857</v>
       </c>
       <c r="C32" s="2">
         <f>SUM(C2:C31)</f>
-        <v>1050</v>
+        <v>0</v>
       </c>
       <c r="D32" s="2">
-        <f t="shared" ref="D32" si="0">SUM(D2:D31)</f>
-        <v>0</v>
+        <f t="shared" ref="D32" si="2">SUM(D2:D31)</f>
+        <v>2550</v>
       </c>
       <c r="E32" s="2"/>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C33">
         <f>C32-B32</f>
-        <v>867</v>
+        <v>-1857</v>
+      </c>
+      <c r="D33">
+        <f>D32-B32</f>
+        <v>693</v>
       </c>
     </row>
   </sheetData>
@@ -1487,12 +1537,12 @@
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B32" s="2">
         <f>SUM(B2:B31)</f>
@@ -1516,10 +1566,13 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1545,122 +1598,27 @@
       <c r="C2">
         <v>415</v>
       </c>
+      <c r="D2">
+        <v>468</v>
+      </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3">
-        <v>375</v>
+        <f>B2*14</f>
+        <v>5250</v>
       </c>
       <c r="C3">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4">
-        <v>375</v>
-      </c>
-      <c r="C4">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5">
-        <v>375</v>
-      </c>
-      <c r="C5">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6">
-        <v>375</v>
-      </c>
-      <c r="C6">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7">
-        <v>375</v>
-      </c>
-      <c r="C7">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8">
-        <v>375</v>
-      </c>
-      <c r="C8">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9">
-        <v>375</v>
-      </c>
-      <c r="C9">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10">
-        <v>375</v>
-      </c>
-      <c r="C10">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11">
-        <v>375</v>
-      </c>
-      <c r="C11">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12">
-        <v>375</v>
-      </c>
-      <c r="C12">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13">
-        <v>375</v>
-      </c>
-      <c r="C13">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14">
-        <v>375</v>
-      </c>
-      <c r="C14">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15">
-        <v>375</v>
-      </c>
-      <c r="C15">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16">
-        <v>375</v>
-      </c>
-      <c r="C16">
-        <v>415</v>
+        <f>C2*14</f>
+        <v>5810</v>
+      </c>
+      <c r="D3">
+        <f>D2*14</f>
+        <v>6552</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B32" s="2">
         <f>SUM(B2:B31)</f>
@@ -1672,14 +1630,18 @@
       </c>
       <c r="D32" s="2">
         <f t="shared" ref="D32" si="0">SUM(D2:D31)</f>
-        <v>0</v>
+        <v>7020</v>
       </c>
       <c r="E32" s="2"/>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C33">
         <f>C32-B32</f>
         <v>600</v>
+      </c>
+      <c r="D33">
+        <f>D32-B32</f>
+        <v>1395</v>
       </c>
     </row>
   </sheetData>
@@ -1690,10 +1652,13 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1719,6 +1684,9 @@
       <c r="C2">
         <v>970</v>
       </c>
+      <c r="D2">
+        <v>500</v>
+      </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3">
@@ -1727,6 +1695,10 @@
       <c r="C3">
         <v>970</v>
       </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D13" si="0">B3*2</f>
+        <v>1000</v>
+      </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4">
@@ -1735,6 +1707,10 @@
       <c r="C4">
         <v>970</v>
       </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5">
@@ -1743,6 +1719,9 @@
       <c r="C5">
         <v>970</v>
       </c>
+      <c r="D5">
+        <v>250</v>
+      </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6">
@@ -1751,6 +1730,9 @@
       <c r="C6">
         <v>970</v>
       </c>
+      <c r="D6">
+        <v>250</v>
+      </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7">
@@ -1758,6 +1740,9 @@
       </c>
       <c r="C7">
         <v>970</v>
+      </c>
+      <c r="D7">
+        <v>250</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
@@ -1767,6 +1752,10 @@
       <c r="C8">
         <v>970</v>
       </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9">
@@ -1775,6 +1764,9 @@
       <c r="C9">
         <v>970</v>
       </c>
+      <c r="D9">
+        <v>500</v>
+      </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10">
@@ -1783,6 +1775,10 @@
       <c r="C10">
         <v>970</v>
       </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>2800</v>
+      </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11">
@@ -1791,6 +1787,10 @@
       <c r="C11">
         <v>970</v>
       </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>2800</v>
+      </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12">
@@ -1799,6 +1799,10 @@
       <c r="C12">
         <v>970</v>
       </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13">
@@ -1807,10 +1811,13 @@
       <c r="C13">
         <v>970</v>
       </c>
+      <c r="D13">
+        <v>250</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B32" s="2">
         <f>SUM(B2:B31)</f>
@@ -1821,15 +1828,19 @@
         <v>11640</v>
       </c>
       <c r="D32" s="2">
-        <f t="shared" ref="D32" si="0">SUM(D2:D31)</f>
-        <v>0</v>
+        <f t="shared" ref="D32" si="1">SUM(D2:D31)</f>
+        <v>11600</v>
       </c>
       <c r="E32" s="2"/>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C33">
         <f>C32-B32</f>
         <v>6008</v>
+      </c>
+      <c r="D33">
+        <f>D32-B32</f>
+        <v>5968</v>
       </c>
     </row>
   </sheetData>
@@ -1841,11 +1852,13 @@
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <tabColor theme="0" tint="-0.34998626667073579"/>
+    <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1864,17 +1877,23 @@
       </c>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>425</v>
+      </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="D2">
+        <v>1190</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B32" s="2">
         <f>SUM(B2:B31)</f>
-        <v>0</v>
+        <v>425</v>
       </c>
       <c r="C32" s="2">
         <f>SUM(C2:C31)</f>
@@ -1882,9 +1901,15 @@
       </c>
       <c r="D32" s="2">
         <f t="shared" ref="D32" si="0">SUM(D2:D31)</f>
-        <v>0</v>
+        <v>1190</v>
       </c>
       <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <f>D32-B32</f>
+        <v>765</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1919,12 +1944,12 @@
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B32" s="2">
         <f>SUM(B2:B31)</f>
@@ -1973,12 +1998,12 @@
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B32" s="2">
         <f>SUM(B2:B31)</f>
@@ -2005,18 +2030,16 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B1" s="2">
         <v>2.2050000000000001</v>
       </c>
@@ -2026,11 +2049,8 @@
       <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>250</v>
       </c>
@@ -2040,11 +2060,8 @@
       <c r="D2">
         <v>375</v>
       </c>
-      <c r="G2">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>250</v>
       </c>
@@ -2054,11 +2071,8 @@
       <c r="D3">
         <v>375</v>
       </c>
-      <c r="G3">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>250</v>
       </c>
@@ -2068,11 +2082,8 @@
       <c r="D4">
         <v>375</v>
       </c>
-      <c r="G4">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>250</v>
       </c>
@@ -2082,11 +2093,8 @@
       <c r="D5">
         <v>375</v>
       </c>
-      <c r="G5">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>250</v>
       </c>
@@ -2096,11 +2104,8 @@
       <c r="D6">
         <v>375</v>
       </c>
-      <c r="G6">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>250</v>
       </c>
@@ -2110,20 +2115,17 @@
       <c r="D7">
         <v>375</v>
       </c>
-      <c r="G7">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B32" s="2">
         <f>SUM(B2:B31)</f>
         <v>1500</v>
       </c>
       <c r="C32" s="2">
-        <f t="shared" ref="C32:G32" si="0">SUM(C2:C31)</f>
+        <f t="shared" ref="C32:D32" si="0">SUM(C2:C31)</f>
         <v>3000</v>
       </c>
       <c r="D32" s="2">
@@ -2131,11 +2133,6 @@
         <v>2250</v>
       </c>
       <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2">
-        <f t="shared" si="0"/>
-        <v>2100</v>
-      </c>
     </row>
     <row r="33" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D33">
@@ -2154,18 +2151,16 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B1" s="2">
         <v>2.2050000000000001</v>
       </c>
@@ -2176,12 +2171,8 @@
         <v>1</v>
       </c>
       <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>220</v>
       </c>
@@ -2189,13 +2180,10 @@
         <v>250</v>
       </c>
       <c r="D2">
-        <v>220</v>
-      </c>
-      <c r="G2">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>88</v>
       </c>
@@ -2205,11 +2193,8 @@
       <c r="D3">
         <v>88</v>
       </c>
-      <c r="G3">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>220</v>
       </c>
@@ -2217,13 +2202,10 @@
         <v>250</v>
       </c>
       <c r="D4">
-        <v>220</v>
-      </c>
-      <c r="G4">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>55</v>
       </c>
@@ -2233,11 +2215,8 @@
       <c r="D5">
         <v>55</v>
       </c>
-      <c r="G5">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>220</v>
       </c>
@@ -2245,13 +2224,10 @@
         <v>250</v>
       </c>
       <c r="D6">
-        <v>220</v>
-      </c>
-      <c r="G6">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>55</v>
       </c>
@@ -2261,11 +2237,8 @@
       <c r="D7">
         <v>55</v>
       </c>
-      <c r="G7">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>55</v>
       </c>
@@ -2275,11 +2248,8 @@
       <c r="D8">
         <v>55</v>
       </c>
-      <c r="G8">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>55</v>
       </c>
@@ -2289,11 +2259,8 @@
       <c r="D9">
         <v>55</v>
       </c>
-      <c r="G9">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>88</v>
       </c>
@@ -2303,11 +2270,8 @@
       <c r="D10">
         <v>88</v>
       </c>
-      <c r="G10">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>220</v>
       </c>
@@ -2315,13 +2279,10 @@
         <v>250</v>
       </c>
       <c r="D11">
-        <v>220</v>
-      </c>
-      <c r="G11">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>220</v>
       </c>
@@ -2329,13 +2290,10 @@
         <v>250</v>
       </c>
       <c r="D12">
-        <v>220</v>
-      </c>
-      <c r="G12">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>220</v>
       </c>
@@ -2343,13 +2301,10 @@
         <v>250</v>
       </c>
       <c r="D13">
-        <v>220</v>
-      </c>
-      <c r="G13">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>88</v>
       </c>
@@ -2359,11 +2314,8 @@
       <c r="D14">
         <v>88</v>
       </c>
-      <c r="G14">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>220</v>
       </c>
@@ -2371,13 +2323,10 @@
         <v>250</v>
       </c>
       <c r="D15">
-        <v>220</v>
-      </c>
-      <c r="G15">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>220</v>
       </c>
@@ -2385,13 +2334,10 @@
         <v>250</v>
       </c>
       <c r="D16">
-        <v>220</v>
-      </c>
-      <c r="G16">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>55</v>
       </c>
@@ -2401,11 +2347,8 @@
       <c r="D17">
         <v>55</v>
       </c>
-      <c r="G17">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>220</v>
       </c>
@@ -2413,13 +2356,10 @@
         <v>250</v>
       </c>
       <c r="D18">
-        <v>220</v>
-      </c>
-      <c r="G18">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>88</v>
       </c>
@@ -2429,11 +2369,8 @@
       <c r="D19">
         <v>88</v>
       </c>
-      <c r="G19">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>88</v>
       </c>
@@ -2443,11 +2380,8 @@
       <c r="D20">
         <v>88</v>
       </c>
-      <c r="G20">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>55</v>
       </c>
@@ -2457,11 +2391,8 @@
       <c r="D21">
         <v>55</v>
       </c>
-      <c r="G21">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>550</v>
       </c>
@@ -2471,11 +2402,8 @@
       <c r="D22">
         <v>750</v>
       </c>
-      <c r="G22">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>550</v>
       </c>
@@ -2485,11 +2413,8 @@
       <c r="D23">
         <v>750</v>
       </c>
-      <c r="G23">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>237.6</v>
       </c>
@@ -2497,13 +2422,10 @@
         <v>500</v>
       </c>
       <c r="D24">
-        <v>500</v>
-      </c>
-      <c r="G24">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>550</v>
       </c>
@@ -2511,13 +2433,10 @@
         <v>550</v>
       </c>
       <c r="D25">
-        <v>750</v>
-      </c>
-      <c r="G25">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>550</v>
       </c>
@@ -2525,13 +2444,10 @@
         <v>550</v>
       </c>
       <c r="D26">
-        <v>750</v>
-      </c>
-      <c r="G26">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>237.6</v>
       </c>
@@ -2541,11 +2457,8 @@
       <c r="D27">
         <v>500</v>
       </c>
-      <c r="G27">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>237.6</v>
       </c>
@@ -2555,11 +2468,8 @@
       <c r="D28">
         <v>500</v>
       </c>
-      <c r="G28">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>237.6</v>
       </c>
@@ -2569,11 +2479,8 @@
       <c r="D29">
         <v>500</v>
       </c>
-      <c r="G29">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>237.6</v>
       </c>
@@ -2583,37 +2490,29 @@
       <c r="D30">
         <v>500</v>
       </c>
-      <c r="G30">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B32" s="2">
         <f>SUM(B2:B31)</f>
         <v>6138.0000000000018</v>
       </c>
       <c r="C32" s="2">
-        <f t="shared" ref="C32:G32" si="0">SUM(C2:C31)</f>
+        <f t="shared" ref="C32:D32" si="0">SUM(C2:C31)</f>
         <v>8385</v>
       </c>
       <c r="D32" s="2">
         <f t="shared" si="0"/>
-        <v>8250</v>
+        <v>8270</v>
       </c>
       <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2">
-        <f t="shared" si="0"/>
-        <v>7135</v>
-      </c>
     </row>
     <row r="33" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D33">
         <f>D32-B32</f>
-        <v>2111.9999999999982</v>
+        <v>2131.9999999999982</v>
       </c>
     </row>
   </sheetData>
@@ -2630,7 +2529,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2739,7 +2638,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B32" s="2">
         <f>SUM(B2:B31)</f>
@@ -2770,9 +2669,9 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <tabColor theme="0" tint="-0.34998626667073579"/>
+    <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2793,17 +2692,159 @@
       </c>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>225</v>
+      </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="D2">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>900</v>
+      </c>
+      <c r="D3">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>900</v>
+      </c>
+      <c r="D4">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>225</v>
+      </c>
+      <c r="D5">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>900</v>
+      </c>
+      <c r="D6">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>900</v>
+      </c>
+      <c r="D7">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>225</v>
+      </c>
+      <c r="D8">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>225</v>
+      </c>
+      <c r="D9">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>225</v>
+      </c>
+      <c r="D10">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>900</v>
+      </c>
+      <c r="D11">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>225</v>
+      </c>
+      <c r="D12">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>225</v>
+      </c>
+      <c r="D13">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>900</v>
+      </c>
+      <c r="D14">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>900</v>
+      </c>
+      <c r="D15">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>900</v>
+      </c>
+      <c r="D16">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>900</v>
+      </c>
+      <c r="D17">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>900</v>
+      </c>
+      <c r="D18">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>225</v>
+      </c>
+      <c r="D19">
+        <v>250</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B32" s="2">
         <f>SUM(B2:B31)</f>
-        <v>0</v>
+        <v>10800</v>
       </c>
       <c r="C32" s="2">
         <f t="shared" ref="C32:D32" si="0">SUM(C2:C31)</f>
@@ -2811,9 +2852,15 @@
       </c>
       <c r="D32" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>11300</v>
       </c>
       <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <f>D32-B32</f>
+        <v>500</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2824,63 +2871,12 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <tabColor theme="0" tint="-0.34998626667073579"/>
+    <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:E32"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B1" s="2">
-        <v>2.2050000000000001</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B32" s="2">
-        <f>SUM(B2:B31)</f>
-        <v>0</v>
-      </c>
-      <c r="C32" s="2">
-        <f t="shared" ref="C32:D32" si="0">SUM(C2:C31)</f>
-        <v>0</v>
-      </c>
-      <c r="D32" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E32" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2900,53 +2896,70 @@
       </c>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>28</v>
+      <c r="B2">
+        <v>1400</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>26</v>
+      </c>
+      <c r="D2">
+        <v>1500</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3">
-        <v>216</v>
-      </c>
-      <c r="C3">
-        <v>223</v>
+        <v>1400</v>
+      </c>
+      <c r="D3">
+        <v>1500</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4">
-        <f>B3*84</f>
-        <v>18144</v>
-      </c>
-      <c r="C4">
-        <f>C3*84</f>
-        <v>18732</v>
+        <v>1400</v>
+      </c>
+      <c r="D4">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1400</v>
+      </c>
+      <c r="D5">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>1400</v>
+      </c>
+      <c r="D6">
+        <v>1500</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B32" s="2">
         <f>SUM(B2:B31)</f>
-        <v>18360</v>
+        <v>7000</v>
       </c>
       <c r="C32" s="2">
-        <f>SUM(C2:C31)</f>
-        <v>18955</v>
+        <f t="shared" ref="C32:D32" si="0">SUM(C2:C31)</f>
+        <v>0</v>
       </c>
       <c r="D32" s="2">
-        <f t="shared" ref="D32" si="0">SUM(D2:D31)</f>
-        <v>0</v>
+        <f>SUM(D2:D31)</f>
+        <v>7500</v>
       </c>
       <c r="E32" s="2"/>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C33">
-        <f>C32-B32</f>
-        <v>595</v>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <f>D32-B32</f>
+        <v>500</v>
       </c>
     </row>
   </sheetData>
@@ -2955,12 +2968,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2981,10 +2997,104 @@
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>216</v>
+      </c>
+      <c r="C3">
+        <v>223</v>
+      </c>
+      <c r="D3">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <f>B3*84</f>
+        <v>18144</v>
+      </c>
+      <c r="C4">
+        <f>C3*84</f>
+        <v>18732</v>
+      </c>
+      <c r="D4">
+        <f>D3*84</f>
+        <v>19404</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" s="2">
+        <f>SUM(B2:B31)</f>
+        <v>18360</v>
+      </c>
+      <c r="C32" s="2">
+        <f>SUM(C2:C31)</f>
+        <v>18955</v>
+      </c>
+      <c r="D32" s="2">
+        <f t="shared" ref="D32" si="0">SUM(D2:D31)</f>
+        <v>19635</v>
+      </c>
+      <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <f>C32-B32</f>
+        <v>595</v>
+      </c>
+      <c r="D33">
+        <f>D32-B32</f>
+        <v>1275</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
+  <dimension ref="A1:E33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="2">
+        <v>2.2050000000000001</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
@@ -2994,6 +3104,10 @@
       <c r="C3">
         <v>100</v>
       </c>
+      <c r="D3">
+        <f>B3*3</f>
+        <v>60</v>
+      </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4">
@@ -3002,6 +3116,10 @@
       <c r="C4">
         <v>100</v>
       </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D24" si="0">B4*3</f>
+        <v>60</v>
+      </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5">
@@ -3010,6 +3128,9 @@
       <c r="C5">
         <v>100</v>
       </c>
+      <c r="D5">
+        <v>25</v>
+      </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6">
@@ -3018,6 +3139,10 @@
       <c r="C6">
         <v>100</v>
       </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7">
@@ -3026,6 +3151,10 @@
       <c r="C7">
         <v>100</v>
       </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8">
@@ -3034,6 +3163,9 @@
       <c r="C8">
         <v>100</v>
       </c>
+      <c r="D8">
+        <v>25</v>
+      </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9">
@@ -3042,6 +3174,10 @@
       <c r="C9">
         <v>100</v>
       </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10">
@@ -3050,6 +3186,9 @@
       <c r="C10">
         <v>100</v>
       </c>
+      <c r="D10">
+        <v>25</v>
+      </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11">
@@ -3058,6 +3197,10 @@
       <c r="C11">
         <v>100</v>
       </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12">
@@ -3066,6 +3209,10 @@
       <c r="C12">
         <v>100</v>
       </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13">
@@ -3074,6 +3221,10 @@
       <c r="C13">
         <v>100</v>
       </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14">
@@ -3082,6 +3233,10 @@
       <c r="C14">
         <v>100</v>
       </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15">
@@ -3090,6 +3245,10 @@
       <c r="C15">
         <v>100</v>
       </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16">
@@ -3098,6 +3257,10 @@
       <c r="C16">
         <v>100</v>
       </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18">
@@ -3106,6 +3269,10 @@
       <c r="C18">
         <v>100</v>
       </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19">
@@ -3114,6 +3281,10 @@
       <c r="C19">
         <v>100</v>
       </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20">
@@ -3122,6 +3293,10 @@
       <c r="C20">
         <v>100</v>
       </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21">
@@ -3130,6 +3305,10 @@
       <c r="C21">
         <v>100</v>
       </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22">
@@ -3138,6 +3317,10 @@
       <c r="C22">
         <v>100</v>
       </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23">
@@ -3146,6 +3329,10 @@
       <c r="C23">
         <v>100</v>
       </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24">
@@ -3154,10 +3341,14 @@
       <c r="C24">
         <v>100</v>
       </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B32" s="2">
         <f>SUM(B2:B31)</f>
@@ -3168,15 +3359,19 @@
         <v>2100</v>
       </c>
       <c r="D32" s="2">
-        <f t="shared" ref="D32" si="0">SUM(D2:D31)</f>
-        <v>0</v>
+        <f t="shared" ref="D32" si="1">SUM(D2:D31)</f>
+        <v>1515</v>
       </c>
       <c r="E32" s="2"/>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C33">
         <f>C32-B32</f>
         <v>1582.5</v>
+      </c>
+      <c r="D33">
+        <f>D32-B32</f>
+        <v>997.5</v>
       </c>
     </row>
   </sheetData>
@@ -3192,7 +3387,9 @@
   </sheetPr>
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3212,12 +3409,15 @@
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B32" s="2">
         <f>SUM(B2:B31)</f>

</xml_diff>